<commit_message>
update for 3.23 Affliction
</commit_message>
<xml_diff>
--- a/src/sextant_mapping.xlsx
+++ b/src/sextant_mapping.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="290">
   <si>
     <t>sextant /142 ⍟</t>
   </si>
@@ -742,22 +742,6 @@
 15 uses remaining</t>
   </si>
   <si>
-    <t>Catalysts dropped by Metamorphs in your Maps are Duplicated
-Metamorphs in your Maps have 100% more Life
-3 uses remaining</t>
-  </si>
-  <si>
-    <t>Catalysts dropped by Metamorphs are duplicated</t>
-  </si>
-  <si>
-    <t>enchant.stat_3011365432</t>
-  </si>
-  <si>
-    <t>Catalysts dropped by Metamorphs in your Maps are Duplicated
-Metamorphs in your Maps have 100% more Life
-15 uses remaining</t>
-  </si>
-  <si>
     <t>Oils found in your Maps are 1 tier higher
 Cost of Building and Upgrading Blight Towers in your Maps is doubled
 3 uses remaining</t>
@@ -1078,17 +1062,17 @@
 15 uses remaining</t>
   </si>
   <si>
-    <t>Area contains Metamorph Monsters
+    <t>Your Maps contain an Ultimatum Encounter
 3 uses remaining</t>
   </si>
   <si>
-    <t>Area contains Metamorph Monsters</t>
-  </si>
-  <si>
-    <t>enchant.stat_1994562755</t>
-  </si>
-  <si>
-    <t>Area contains Metamorph Monsters
+    <t>Areas contain an Ultimatum Encounter</t>
+  </si>
+  <si>
+    <t>enchant.stat_2055257822</t>
+  </si>
+  <si>
+    <t>Your Maps contain an Ultimatum Encounter
 15 uses remaining</t>
   </si>
   <si>
@@ -3090,7 +3074,9 @@
       <c r="C99" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="D99" s="8"/>
+      <c r="D99" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="E99" s="7" t="s">
         <v>12</v>
       </c>
@@ -3105,7 +3091,9 @@
       <c r="C100" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="D100" s="5"/>
+      <c r="D100" s="4" t="s">
+        <v>147</v>
+      </c>
       <c r="E100" s="4" t="s">
         <v>12</v>
       </c>
@@ -3115,13 +3103,13 @@
         <v>203</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D101" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E101" s="7" t="s">
         <v>12</v>
@@ -3129,16 +3117,16 @@
     </row>
     <row r="102">
       <c r="A102" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>147</v>
+        <v>70</v>
       </c>
       <c r="E102" s="4" t="s">
         <v>12</v>
@@ -3146,16 +3134,16 @@
     </row>
     <row r="103">
       <c r="A103" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D103" s="7" t="s">
-        <v>67</v>
+        <v>147</v>
       </c>
       <c r="E103" s="7" t="s">
         <v>12</v>
@@ -3163,16 +3151,16 @@
     </row>
     <row r="104">
       <c r="A104" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E104" s="4" t="s">
         <v>12</v>
@@ -3180,17 +3168,15 @@
     </row>
     <row r="105">
       <c r="A105" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C105" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="B105" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="C105" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="D105" s="7" t="s">
-        <v>147</v>
-      </c>
+      <c r="D105" s="8"/>
       <c r="E105" s="7" t="s">
         <v>12</v>
       </c>
@@ -3200,14 +3186,12 @@
         <v>210</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="D106" s="4" t="s">
-        <v>67</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="D106" s="5"/>
       <c r="E106" s="4" t="s">
         <v>12</v>
       </c>
@@ -3282,14 +3266,16 @@
       <c r="C111" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="D111" s="8"/>
+      <c r="D111" s="7" t="s">
+        <v>222</v>
+      </c>
       <c r="E111" s="7" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B112" s="4" t="s">
         <v>220</v>
@@ -3297,23 +3283,25 @@
       <c r="C112" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="D112" s="5"/>
+      <c r="D112" s="4" t="s">
+        <v>224</v>
+      </c>
       <c r="E112" s="4" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="6" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D113" s="7" t="s">
-        <v>226</v>
+        <v>28</v>
       </c>
       <c r="E113" s="7" t="s">
         <v>26</v>
@@ -3321,16 +3309,16 @@
     </row>
     <row r="114">
       <c r="A114" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C114" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="B114" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="C114" s="4" t="s">
-        <v>225</v>
-      </c>
       <c r="D114" s="4" t="s">
-        <v>228</v>
+        <v>92</v>
       </c>
       <c r="E114" s="4" t="s">
         <v>26</v>
@@ -3364,7 +3352,7 @@
         <v>231</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>92</v>
+        <v>233</v>
       </c>
       <c r="E116" s="4" t="s">
         <v>26</v>
@@ -3372,47 +3360,43 @@
     </row>
     <row r="117">
       <c r="A117" s="6" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="D117" s="7" t="s">
-        <v>28</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="D117" s="8"/>
       <c r="E117" s="7" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="D118" s="4" t="s">
-        <v>237</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="D118" s="5"/>
       <c r="E118" s="4" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="6" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D119" s="8"/>
       <c r="E119" s="7" t="s">
@@ -3421,13 +3405,13 @@
     </row>
     <row r="120">
       <c r="A120" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D120" s="5"/>
       <c r="E120" s="4" t="s">
@@ -3436,32 +3420,32 @@
     </row>
     <row r="121">
       <c r="A121" s="6" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D121" s="8"/>
       <c r="E121" s="7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B122" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="C122" s="4" t="s">
         <v>248</v>
-      </c>
-      <c r="C122" s="4" t="s">
-        <v>249</v>
       </c>
       <c r="D122" s="5"/>
       <c r="E122" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="123">
@@ -3476,7 +3460,7 @@
       </c>
       <c r="D123" s="8"/>
       <c r="E123" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="124">
@@ -3484,43 +3468,47 @@
         <v>253</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="D124" s="5"/>
+        <v>255</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>256</v>
+      </c>
       <c r="E124" s="4" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="B125" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="B125" s="7" t="s">
+      <c r="C125" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="C125" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="D125" s="8"/>
+      <c r="D125" s="7" t="s">
+        <v>224</v>
+      </c>
       <c r="E125" s="7" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E126" s="4" t="s">
         <v>26</v>
@@ -3531,13 +3519,13 @@
         <v>261</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D127" s="7" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E127" s="7" t="s">
         <v>26</v>
@@ -3553,11 +3541,9 @@
       <c r="C128" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="D128" s="4" t="s">
-        <v>260</v>
-      </c>
+      <c r="D128" s="5"/>
       <c r="E128" s="4" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="129">
@@ -3570,11 +3556,9 @@
       <c r="C129" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="D129" s="7" t="s">
-        <v>228</v>
-      </c>
+      <c r="D129" s="8"/>
       <c r="E129" s="7" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="130">
@@ -3758,34 +3742,18 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="B142" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="C142" s="4" t="s">
-        <v>292</v>
-      </c>
+      <c r="A142" s="13"/>
+      <c r="B142" s="5"/>
+      <c r="C142" s="5"/>
       <c r="D142" s="5"/>
-      <c r="E142" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="E142" s="5"/>
     </row>
     <row r="143">
-      <c r="A143" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="B143" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="C143" s="7" t="s">
-        <v>292</v>
-      </c>
+      <c r="A143" s="14"/>
+      <c r="B143" s="8"/>
+      <c r="C143" s="8"/>
       <c r="D143" s="8"/>
-      <c r="E143" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="E143" s="8"/>
     </row>
     <row r="144">
       <c r="A144" s="13"/>
@@ -4166,18 +4134,18 @@
       <c r="E197" s="8"/>
     </row>
     <row r="198">
-      <c r="A198" s="13"/>
-      <c r="B198" s="5"/>
-      <c r="C198" s="5"/>
-      <c r="D198" s="5"/>
-      <c r="E198" s="5"/>
+      <c r="A198" s="15"/>
+      <c r="B198" s="15"/>
+      <c r="C198" s="15"/>
+      <c r="D198" s="15"/>
+      <c r="E198" s="15"/>
     </row>
     <row r="199">
-      <c r="A199" s="14"/>
-      <c r="B199" s="8"/>
-      <c r="C199" s="8"/>
-      <c r="D199" s="8"/>
-      <c r="E199" s="8"/>
+      <c r="A199" s="15"/>
+      <c r="B199" s="15"/>
+      <c r="C199" s="15"/>
+      <c r="D199" s="15"/>
+      <c r="E199" s="15"/>
     </row>
     <row r="200">
       <c r="A200" s="15"/>
@@ -9771,20 +9739,6 @@
       <c r="C998" s="15"/>
       <c r="D998" s="15"/>
       <c r="E998" s="15"/>
-    </row>
-    <row r="999">
-      <c r="A999" s="15"/>
-      <c r="B999" s="15"/>
-      <c r="C999" s="15"/>
-      <c r="D999" s="15"/>
-      <c r="E999" s="15"/>
-    </row>
-    <row r="1000">
-      <c r="A1000" s="15"/>
-      <c r="B1000" s="15"/>
-      <c r="C1000" s="15"/>
-      <c r="D1000" s="15"/>
-      <c r="E1000" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>